<commit_message>
Pre-projeto final para residência técnica
</commit_message>
<xml_diff>
--- a/Projeto_Final/Documentacao/Cronograma.xlsx
+++ b/Projeto_Final/Documentacao/Cronograma.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RepositorioGit\Residencia\Projeto_Final\Hardware\Documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RepositorioGit\Residencia\Projeto_Final\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12211EA-F845-41E0-9DC1-BCC76CBB1EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CDFB9E-33DC-48B6-BFC5-5A2D88881410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AF4A3E11-11B9-4F2F-88E4-D265585E69ED}"/>
   </bookViews>
@@ -75,19 +75,6 @@
     <t>CRONOGRAMA - PROJETO FINAL Embarcatech</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Residential Energy Monitoring System - </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <rFont val="Space Age"/>
-      </rPr>
-      <t>REMSYS</t>
-    </r>
-  </si>
-  <si>
     <t>Semana 8</t>
   </si>
   <si>
@@ -107,6 +94,9 @@
   </si>
   <si>
     <t>Data prevista para término:</t>
+  </si>
+  <si>
+    <t>Sistema IoT para Medição e Análise de Consumo Elétrico Residencial</t>
   </si>
 </sst>
 </file>
@@ -117,14 +107,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -153,12 +135,22 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
-      <name val="Space Age"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -235,44 +227,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,286 +580,265 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M12"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.7109375" customWidth="1"/>
-    <col min="2" max="16" width="10.7109375" customWidth="1"/>
+    <col min="2" max="13" width="12.7109375" customWidth="1"/>
+    <col min="14" max="16" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
+      <c r="A3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="14">
+      <c r="A4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="8">
         <v>45964</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="14">
+      <c r="C4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="8">
         <f>B4+12*7</f>
         <v>46048</v>
       </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="M5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+    </row>
+    <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+    </row>
+    <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+    </row>
+    <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
     </row>
     <row r="21" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O21" s="5"/>
+      <c r="O21" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>